<commit_message>
king and pawn pseudo and valid move generation routines
</commit_message>
<xml_diff>
--- a/masks.xlsx
+++ b/masks.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>0000000000000000000000000000000000000000000000000000000011111111</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t>bit:</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>&lt;</t>
   </si>
 </sst>
 </file>
@@ -448,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB25"/>
+  <dimension ref="A1:AB30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1254,6 +1260,28 @@
         <v>15</v>
       </c>
     </row>
+    <row r="29" spans="4:19" x14ac:dyDescent="0.3">
+      <c r="H29">
+        <v>28</v>
+      </c>
+      <c r="I29" t="s">
+        <v>18</v>
+      </c>
+      <c r="J29">
+        <v>27</v>
+      </c>
+      <c r="N29" t="s">
+        <v>19</v>
+      </c>
+      <c r="O29">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="4:19" x14ac:dyDescent="0.3">
+      <c r="H30">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
game loop and ascii renderer
</commit_message>
<xml_diff>
--- a/masks.xlsx
+++ b/masks.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Coding\dama-ai\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emanuel\Documents\GitHub\dama-ai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41457086-518B-4C3A-A69E-84B6CDAA9B23}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11835" yWindow="1170" windowWidth="13575" windowHeight="14205" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11832" yWindow="1176" windowWidth="13572" windowHeight="14208"/>
   </bookViews>
   <sheets>
     <sheet name="board" sheetId="1" r:id="rId1"/>
     <sheet name="benchmarks" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -115,7 +114,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -482,16 +481,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB30"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="5.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <f t="shared" ref="A1:A6" si="0">A2+8</f>
         <v>56</v>
@@ -569,7 +568,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -602,52 +601,68 @@
         <f t="shared" si="7"/>
         <v>55</v>
       </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
+      <c r="J2" s="1">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1">
+        <v>1</v>
+      </c>
+      <c r="L2" s="1">
+        <v>1</v>
+      </c>
+      <c r="M2" s="1">
+        <v>1</v>
+      </c>
+      <c r="N2" s="1">
+        <v>1</v>
+      </c>
+      <c r="O2" s="1">
+        <v>1</v>
+      </c>
+      <c r="P2" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>1</v>
+      </c>
       <c r="S2" s="2">
         <f t="shared" ref="S2:S6" si="8">Q2</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T2" s="2">
         <f t="shared" ref="T2:T6" si="9">P2</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U2" s="2">
         <f t="shared" ref="U2:U6" si="10">O2</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V2" s="2">
         <f t="shared" ref="V2:V6" si="11">N2</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W2" s="2">
         <f t="shared" ref="W2:W6" si="12">M2</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X2" s="2">
         <f t="shared" ref="X2:X6" si="13">L2</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y2" s="2">
         <f t="shared" ref="Y2:Y6" si="14">K2</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z2" s="2">
         <f t="shared" ref="Z2:Z6" si="15">J2</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB2" t="str">
         <f t="shared" ref="AB2:AB8" si="16">_xlfn.CONCAT(S2:Z2)</f>
-        <v>00000000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+        <v>11111111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -680,52 +695,68 @@
         <f t="shared" si="7"/>
         <v>47</v>
       </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
+      <c r="J3" s="1">
+        <v>1</v>
+      </c>
+      <c r="K3" s="1">
+        <v>1</v>
+      </c>
+      <c r="L3" s="1">
+        <v>1</v>
+      </c>
+      <c r="M3" s="1">
+        <v>1</v>
+      </c>
+      <c r="N3" s="1">
+        <v>1</v>
+      </c>
+      <c r="O3" s="1">
+        <v>1</v>
+      </c>
+      <c r="P3" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>1</v>
+      </c>
       <c r="S3" s="2">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T3" s="2">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U3" s="2">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V3" s="2">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W3" s="2">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X3" s="2">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y3" s="2">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z3" s="2">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB3" t="str">
         <f t="shared" si="16"/>
-        <v>00000000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+        <v>11111111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -803,7 +834,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -881,7 +912,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -959,7 +990,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <f>A8+8</f>
         <v>8</v>
@@ -1037,7 +1068,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>0</v>
       </c>
@@ -1107,21 +1138,21 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>17</v>
       </c>
       <c r="C11" t="str">
         <f>_xlfn.CONCAT(AB1:AB8)</f>
-        <v>0000000000000000000000000000000000000000000000000000000000000000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+        <v>0000000011111111111111110000000000000000000000000000000000000000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D18">
         <v>0</v>
       </c>
@@ -1135,7 +1166,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D19">
         <v>1</v>
       </c>
@@ -1149,7 +1180,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D20">
         <v>2</v>
       </c>
@@ -1163,7 +1194,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D21">
         <v>3</v>
       </c>
@@ -1177,7 +1208,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D22">
         <v>4</v>
       </c>
@@ -1191,7 +1222,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D23">
         <v>5</v>
       </c>
@@ -1205,7 +1236,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D24">
         <v>6</v>
       </c>
@@ -1219,7 +1250,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D25">
         <v>7</v>
       </c>
@@ -1233,7 +1264,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:19" x14ac:dyDescent="0.3">
       <c r="H29">
         <v>28</v>
       </c>
@@ -1250,7 +1281,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:19" x14ac:dyDescent="0.3">
       <c r="H30">
         <v>35</v>
       </c>
@@ -1261,24 +1292,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5977848-EEC3-43EF-ACF9-FC8F0A16A4FC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>20</v>
       </c>
@@ -1298,7 +1329,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -1320,7 +1351,7 @@
         <v>0.22222222222222221</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -1342,7 +1373,7 @@
         <v>16.164383561643834</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1364,7 +1395,7 @@
         <v>1.5732394366197184</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -1386,7 +1417,7 @@
         <v>0.19317496683950319</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -1408,7 +1439,7 @@
         <v>5.400010877250231E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>5</v>
       </c>

</xml_diff>